<commit_message>
excel functions relative ranges
</commit_message>
<xml_diff>
--- a/Tests/WebVella.DocumentTemplates.Tests/Files/TemplateFunction-SUM-1.xlsx
+++ b/Tests/WebVella.DocumentTemplates.Tests/Files/TemplateFunction-SUM-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\WebVella.DocumentTemplates\Tests\WebVella.DocumentTemplates.Tests\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FD809F-598B-4A3B-95F0-C673D27500DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C86615-9B68-466B-B9F2-B4F7664BA1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4452" yWindow="12180" windowWidth="35976" windowHeight="19320" xr2:uid="{249ED8D8-E4C7-4A41-9BC3-D6950499A5E0}"/>
+    <workbookView xWindow="57480" yWindow="12375" windowWidth="29040" windowHeight="15720" xr2:uid="{249ED8D8-E4C7-4A41-9BC3-D6950499A5E0}"/>
   </bookViews>
   <sheets>
     <sheet name="{{name}}" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +77,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -108,10 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,24 +438,24 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:C2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.109375" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -457,7 +466,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>